<commit_message>
Verified that the Diff Check Tool is working
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adcsuf-my.sharepoint.com/personal/duynguyen1993_csu_fullerton_edu/Documents/Work-Related Documents/SCCWRP/Projects/General-Diff-Check/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\PartTimers\DuyNguyen\Projects\General-Diff-Check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC1048BA09987BAC5BDE58E9" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E4C16197-0523-4DF9-AAA9-59BE875F729C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBE8DD4-4C42-4306-9F8C-A1D5ECA31A9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="26235" windowHeight="14895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3165" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -366,7 +366,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>